<commit_message>
Deploying to gh-pages from @ eurovibes/klima@5c535bcd9771f1b051b3730450bd54cc566833c9 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/klima-bom_0.1.xlsx
+++ b/Fabrication/BoM/klima-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
   <si>
     <t>Row</t>
   </si>
@@ -140,6 +140,21 @@
     <t>7</t>
   </si>
   <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>10 kΩ</t>
+  </si>
+  <si>
+    <t>R_Axial_DIN0207_L6.3mm_D2.5mm_P7.62mm_Horizontal</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>SW101</t>
   </si>
   <si>
@@ -152,7 +167,7 @@
     <t>SW_PUSH_6mm</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>U102</t>
@@ -164,7 +179,7 @@
     <t>Aosong_DHT11_5.5x12.0_P2.54mm</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>U101</t>
@@ -697,7 +712,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -720,7 +735,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -732,55 +747,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F4" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -788,16 +803,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1067,7 +1082,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>13</v>
@@ -1079,7 +1094,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>13</v>
@@ -1090,16 +1105,16 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
@@ -1111,12 +1126,44 @@
         <v>13</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1134,10 +1181,11 @@
     <hyperlink ref="G15" r:id="rId7"/>
     <hyperlink ref="G16" r:id="rId8"/>
     <hyperlink ref="G17" r:id="rId9"/>
+    <hyperlink ref="G18" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1154,17 +1202,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/klima@df60b01758793febb80c14a34d83a064e1e387b4 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/klima-bom_0.1.xlsx
+++ b/Fabrication/BoM/klima-bom_0.1.xlsx
@@ -98,7 +98,7 @@
     <t>J101 J102</t>
   </si>
   <si>
-    <t>Conn_02x04_Top_Bottom</t>
+    <t>Conn_02x04_Odd_Even</t>
   </si>
   <si>
     <t>ESP8266-01S</t>
@@ -395,7 +395,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>513398</xdr:colOff>
+      <xdr:colOff>646748</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>43656</xdr:rowOff>
     </xdr:to>
@@ -723,7 +723,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>

</xml_diff>